<commit_message>
Update content with new changes
</commit_message>
<xml_diff>
--- a/generated/Carbon_Footprint_Report.xlsx
+++ b/generated/Carbon_Footprint_Report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="105">
   <si>
     <t>活動數據</t>
   </si>
@@ -59,55 +59,94 @@
     <t>大鋼胚</t>
   </si>
   <si>
+    <t>公斤(kg)</t>
+  </si>
+  <si>
+    <t>鋼胚(電弧爐製程，不分型號)</t>
+  </si>
+  <si>
+    <t>環境部產品碳足跡資訊網</t>
+  </si>
+  <si>
+    <t>鋼胚製造過程沒有盤查，直接套用資料庫係數</t>
+  </si>
+  <si>
+    <t>製造生產階段</t>
+  </si>
+  <si>
+    <t>能源</t>
+  </si>
+  <si>
+    <t>天然氣(NG)</t>
+  </si>
+  <si>
+    <t>立方公尺(m3)</t>
+  </si>
+  <si>
+    <t>天然氣(於固定源使用，2021)</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>台電電力</t>
+  </si>
+  <si>
+    <t>度(kwh)</t>
+  </si>
+  <si>
+    <t>電力碳足跡(2021)</t>
+  </si>
+  <si>
+    <t>黑鐵線</t>
+  </si>
+  <si>
+    <t>生鐵</t>
+  </si>
+  <si>
+    <t>捆包用</t>
+  </si>
+  <si>
+    <t>車用柴油</t>
+  </si>
+  <si>
+    <t>公升(L)</t>
+  </si>
+  <si>
+    <t>柴油(於鐵路運輸與非道路運輸移動源使用，2021)</t>
+  </si>
+  <si>
+    <t>廢棄處理階段</t>
+  </si>
+  <si>
+    <t>排放</t>
+  </si>
+  <si>
+    <t>化糞池逸散</t>
+  </si>
+  <si>
+    <t>kg CO2e</t>
+  </si>
+  <si>
+    <t>化糞池 CO2 排放</t>
+  </si>
+  <si>
     <t>kg</t>
   </si>
   <si>
-    <t>鋼胚(電弧爐製程，不分型號)</t>
-  </si>
-  <si>
-    <t>kg CO2e/kg</t>
-  </si>
-  <si>
-    <t>環境部產品碳足跡資訊網</t>
-  </si>
-  <si>
-    <t>鋼胚製造過程未盤查，直接套用資料庫係數</t>
-  </si>
-  <si>
-    <t>製造生產階段</t>
-  </si>
-  <si>
-    <t>能源</t>
-  </si>
-  <si>
-    <t>天然氣(NG)</t>
-  </si>
-  <si>
-    <t>m3</t>
-  </si>
-  <si>
-    <t>天然氣(於固定源使用，2021)</t>
-  </si>
-  <si>
-    <t>kg CO2e/m3</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>台電電力</t>
-  </si>
-  <si>
-    <t>kwh</t>
-  </si>
-  <si>
-    <t>電力碳足跡(2021)</t>
-  </si>
-  <si>
-    <t>kg CO2e/kwh</t>
-  </si>
-  <si>
-    <t>黑鐵線</t>
+    <t>放流水</t>
+  </si>
+  <si>
+    <t>廢(污)水處理服務(高雄市楠梓污水處理廠)</t>
+  </si>
+  <si>
+    <t>資源</t>
+  </si>
+  <si>
+    <t>自來水</t>
+  </si>
+  <si>
+    <t>臺灣自來水(2020)</t>
   </si>
   <si>
     <t>輔助項</t>
@@ -116,12 +155,45 @@
     <t>防腐防垢抑制劑</t>
   </si>
   <si>
+    <t>腐蝕抑制劑</t>
+  </si>
+  <si>
+    <t>依照產品成分標示自行組合係數</t>
+  </si>
+  <si>
+    <t>運輸</t>
+  </si>
+  <si>
+    <t>原料階段來料運輸-陸運(TKM)</t>
+  </si>
+  <si>
+    <t>延噸公里(tkm)</t>
+  </si>
+  <si>
+    <t>營業大貨車(柴油)</t>
+  </si>
+  <si>
+    <t>一般事業廢棄物</t>
+  </si>
+  <si>
+    <t>一般事業廢棄物掩埋處理服務</t>
+  </si>
+  <si>
+    <t>碳標籤第 2113820001 號 掩埋</t>
+  </si>
+  <si>
+    <t>能源來料運輸-陸運(TKM)</t>
+  </si>
+  <si>
+    <t>營業小貨車(柴油)</t>
+  </si>
+  <si>
+    <t>製造階段廢棄物清除運輸-陸運(TKM)</t>
+  </si>
+  <si>
     <t>毫米(mm)</t>
   </si>
   <si>
-    <t>資源</t>
-  </si>
-  <si>
     <t>公分(cm)</t>
   </si>
   <si>
@@ -137,9 +209,6 @@
     <t>公里(km)</t>
   </si>
   <si>
-    <t>廢棄處理階段</t>
-  </si>
-  <si>
     <t>產品</t>
   </si>
   <si>
@@ -155,9 +224,6 @@
     <t>英寸(in)</t>
   </si>
   <si>
-    <t>排放</t>
-  </si>
-  <si>
     <t>碼(yard)</t>
   </si>
   <si>
@@ -170,9 +236,6 @@
     <t>公克(g)</t>
   </si>
   <si>
-    <t>公斤(kg)</t>
-  </si>
-  <si>
     <t>公噸(mt)</t>
   </si>
   <si>
@@ -182,9 +245,6 @@
     <t>毫升(ml)</t>
   </si>
   <si>
-    <t>公升(L)</t>
-  </si>
-  <si>
     <t>公秉(kl)</t>
   </si>
   <si>
@@ -206,28 +266,16 @@
     <t>立方公分(cm3)</t>
   </si>
   <si>
-    <t>立方公尺(m3)</t>
-  </si>
-  <si>
     <t>立方公里(km3)</t>
   </si>
   <si>
     <t>百萬焦耳(MJ)</t>
   </si>
   <si>
-    <t>度(kwh)</t>
-  </si>
-  <si>
     <t>延人公里(pkm)</t>
   </si>
   <si>
-    <t>延噸公里(tkm)</t>
-  </si>
-  <si>
     <t>g CO2e</t>
-  </si>
-  <si>
-    <t>kg CO2e</t>
   </si>
   <si>
     <t>每平方米‧每小時</t>
@@ -655,7 +703,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L15"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -743,129 +791,469 @@
         <v>0.678</v>
       </c>
       <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>18</v>
-      </c>
-      <c r="L3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
       </c>
       <c r="D4">
         <v>5720</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4">
         <v>52</v>
       </c>
       <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
         <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
       </c>
       <c r="I4">
         <v>2.63</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
       <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>11880</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5">
+        <v>108</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
         <v>27</v>
-      </c>
-      <c r="D5">
-        <v>11748</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5">
-        <v>106.8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" t="s">
-        <v>29</v>
       </c>
       <c r="I5">
         <v>0.606</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>8250</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>75</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6">
+        <v>1.81</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>4015</v>
+      </c>
+      <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7">
+        <v>36.5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
         <v>33</v>
       </c>
-      <c r="D7">
-        <v>229.9</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="I7">
+        <v>3.56</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>1331</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8">
+        <v>12.1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>3861</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>3.51</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9">
+        <v>0.4</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10">
+        <v>4845</v>
+      </c>
+      <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="F7">
+      <c r="F10">
+        <v>4.5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10">
+        <v>0.233</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11">
+        <v>0.561</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>0.00053</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11">
         <v>2.09</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J11" t="s">
         <v>15</v>
       </c>
-      <c r="L7" t="s">
-        <v>26</v>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>0.007035</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12">
+        <v>0.0000063</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12">
+        <v>1.31</v>
+      </c>
+      <c r="J12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13">
+        <v>0.0005005</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>4.55e-7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13">
+        <v>7</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14">
+        <v>0.0008217</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14">
+        <v>7.47e-7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14">
+        <v>5.87</v>
+      </c>
+      <c r="J14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15">
+        <v>0.000715</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15">
+        <v>6.5e-7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15">
+        <v>1.31</v>
+      </c>
+      <c r="J15" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -874,20 +1262,35 @@
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="L1:L2"/>
   </mergeCells>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" sqref="A3:A7">
+  <dataValidations count="10">
+    <dataValidation type="list" allowBlank="1" sqref="A10:A15">
       <formula1>Code!$A$1:$A$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B3:B7">
+    <dataValidation type="list" allowBlank="1" sqref="A3:A15">
+      <formula1>Code!$A$1:$A$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="B10:B15">
       <formula1>Code!$C$1:$C$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E3:E7">
+    <dataValidation type="list" allowBlank="1" sqref="B3:B15">
+      <formula1>Code!$C$1:$C$8</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="E10:E15">
       <formula1>Code!$G$1:$G$46</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G3:G7">
+    <dataValidation type="list" allowBlank="1" sqref="E3:E15">
       <formula1>Code!$G$1:$G$46</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J3:J7">
+    <dataValidation type="list" allowBlank="1" sqref="G10:G15">
+      <formula1>Code!$G$1:$G$46</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="G3:G15">
+      <formula1>Code!$G$1:$G$46</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="J10:J15">
+      <formula1>Code!$G$1:$G$46</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="J3:J15">
       <formula1>Code!$G$1:$G$46</formula1>
     </dataValidation>
   </dataValidations>
@@ -906,547 +1309,547 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="J8" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="J9" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="J12" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="J13" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="J14" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="J15" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="J16" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="J17" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="J18" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G19" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="J19" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="J20" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="J21" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="J22" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="G23" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="J23" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="G24" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="J24" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="G25" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="J25" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="G26" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="J26" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="G27" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="J27" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="G28" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="J28" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="G29" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="J29" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="G30" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="J30" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="G31" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="J31" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="G32" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="J32" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="G33" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="J33" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="G34" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="J34" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="G35" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="J35" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="G36" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="J36" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="G37" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="J37" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="G38" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="J38" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="G39" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="J39" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="G40" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="J40" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="G41" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="J41" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="G42" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="J42" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="G43" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="J43" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="G44" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="J44" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="G45" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="J45" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="G46" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="J46" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>